<commit_message>
update code QLSV 31/5 by Huan
</commit_message>
<xml_diff>
--- a/pages/bang-hoc-phi.xlsx
+++ b/pages/bang-hoc-phi.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Bảng học phí" sheetId="1" r:id="rId4"/>
+    <sheet name="Bảng rèn luyện" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -15,96 +15,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Mã học phí</t>
+    <t>Mã sinh viên</t>
   </si>
   <si>
     <t>Tên sinh viên</t>
   </si>
   <si>
-    <t>Chức vụ</t>
-  </si>
-  <si>
-    <t>Học phí kỳ</t>
-  </si>
-  <si>
-    <t>Số tín chỉ</t>
-  </si>
-  <si>
-    <t>Còn nợ</t>
-  </si>
-  <si>
-    <t>Ngày dóng</t>
-  </si>
-  <si>
-    <t>ML1614090618</t>
+    <t>Học kỳ</t>
+  </si>
+  <si>
+    <t>Năm</t>
+  </si>
+  <si>
+    <t>Tiêu chí 1</t>
+  </si>
+  <si>
+    <t>Tiêu chí 2</t>
+  </si>
+  <si>
+    <t>Tiêu chí 3</t>
+  </si>
+  <si>
+    <t>Tiêu chí 4</t>
+  </si>
+  <si>
+    <t>Tiêu chí 5</t>
+  </si>
+  <si>
+    <t>Tổng điểm</t>
+  </si>
+  <si>
+    <t>Xếp Loại</t>
+  </si>
+  <si>
+    <t>Ngày Xét</t>
+  </si>
+  <si>
+    <t>17D150026</t>
   </si>
   <si>
     <t>Trương Hoàng Vũ</t>
   </si>
   <si>
-    <t>Sinh viên</t>
-  </si>
-  <si>
-    <t>3,960,000vnđ</t>
-  </si>
-  <si>
-    <t>1vnđ</t>
-  </si>
-  <si>
-    <t>2021-02-23</t>
-  </si>
-  <si>
-    <t>ML1613899061</t>
-  </si>
-  <si>
-    <t>Trương Huy Huân</t>
-  </si>
-  <si>
-    <t>3,950,000vnđ</t>
-  </si>
-  <si>
-    <t>10,000vnđ</t>
-  </si>
-  <si>
-    <t>2021-02-21</t>
-  </si>
-  <si>
-    <t>ML1614090572</t>
-  </si>
-  <si>
-    <t>ML1614090985</t>
-  </si>
-  <si>
-    <t>0vnđ</t>
-  </si>
-  <si>
-    <t>ML1614090207</t>
-  </si>
-  <si>
-    <t>3,959,999vnđ</t>
-  </si>
-  <si>
-    <t>ML1614089914</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Quý</t>
-  </si>
-  <si>
-    <t>ML1614090031</t>
-  </si>
-  <si>
-    <t>3,959,000vnđ</t>
-  </si>
-  <si>
-    <t>1,000vnđ</t>
-  </si>
-  <si>
-    <t>ML1614091022</t>
+    <t>Kém</t>
+  </si>
+  <si>
+    <t>2021-05-05</t>
   </si>
 </sst>
 </file>
@@ -469,10 +430,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -480,14 +441,19 @@
     <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,213 +478,61 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:13">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="2">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2">
-        <v>11</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="2">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>